<commit_message>
Implemented the merge email
</commit_message>
<xml_diff>
--- a/TestSS.xlsx
+++ b/TestSS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andersonpech/Desktop/PyExcel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ander\Documents\MailMergerWithAttachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95C5E03A-C3FE-2E42-B0E0-C4C50BB56EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B8305C-1F4D-4161-B649-20B4FE671AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="520" windowWidth="28040" windowHeight="16100" xr2:uid="{E8AFDA4E-1DD6-2A45-82E3-89D6DA16F2B0}"/>
+    <workbookView xWindow="3465" yWindow="3450" windowWidth="21600" windowHeight="11385" xr2:uid="{E8AFDA4E-1DD6-2A45-82E3-89D6DA16F2B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,23 +36,31 @@
     <t>Attachment</t>
   </si>
   <si>
-    <t>Eren</t>
-  </si>
-  <si>
-    <t>Mikasa</t>
-  </si>
-  <si>
-    <t>Armin</t>
+    <t>SamplePDF.pdf</t>
+  </si>
+  <si>
+    <t>Enter email</t>
+  </si>
+  <si>
+    <t>Foo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +83,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -394,15 +405,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31EE43F-4B2D-7E44-8E4A-F3FBC71ED74E}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,22 +424,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="andersonpech@gmail.com" xr:uid="{4E1BEE89-219D-4677-924E-F8521594A295}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>